<commit_message>
RESULTS: Changed formatting of table and chart.
</commit_message>
<xml_diff>
--- a/documents/bigprak_ergebnisse.xlsx
+++ b/documents/bigprak_ergebnisse.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\bigdata-kylin-dblp\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>KYLIN</t>
   </si>
@@ -67,6 +67,12 @@
   <si>
     <t>MITTELWERT</t>
   </si>
+  <si>
+    <t>Abfragen</t>
+  </si>
+  <si>
+    <t>Ausführungszeit (in Sekunden)</t>
+  </si>
 </sst>
 </file>
 
@@ -97,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -383,37 +389,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -466,7 +495,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Ausführungszeit</a:t>
+              <a:t>Ausführungszeit/Abfrage (in Sekunden)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -513,7 +542,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$C$2</c:f>
+              <c:f>Tabelle1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -534,7 +563,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$3:$B$12</c:f>
+              <c:f>Tabelle1!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -572,9 +601,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$12</c:f>
+              <c:f>Tabelle1!$C$4:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>177.34299999999999</c:v>
@@ -615,7 +644,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$2</c:f>
+              <c:f>Tabelle1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -636,7 +665,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$B$3:$B$12</c:f>
+              <c:f>Tabelle1!$B$4:$B$13</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -674,9 +703,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$3:$D$12</c:f>
+              <c:f>Tabelle1!$D$4:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>51.33</c:v>
@@ -721,132 +750,137 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="373448288"/>
-        <c:axId val="373447728"/>
+        <c:axId val="84274144"/>
+        <c:axId val="84274704"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$E$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>ERSPARNIS</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$4:$B$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>#-Pub/Autor</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>#-Pub/2015/Autor</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>MAX-Zit/Autor/Pub</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>MAX-Zit/Autor</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>#-Pub/Rahm</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>#-Pub/2015/Rahm</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>MAX-Zit/Pub/Rahm</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>SUM-Zit/Rahm</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>#-Pub/Groß</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>#-Pub/2015/Groß</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$E$4:$E$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>#,##0.00</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>126.01299999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>69.328000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>105.357</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>286.15899999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>70.63000000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>56.046999999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>184.53300000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>53.843000000000004</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>94.222000000000008</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>79.174000000000007</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ERSPARNIS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Tabelle1!$B$3:$B$12</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>#-Pub/Autor</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>#-Pub/2015/Autor</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MAX-Zit/Autor/Pub</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>MAX-Zit/Autor</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>#-Pub/Rahm</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>#-Pub/2015/Rahm</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>MAX-Zit/Pub/Rahm</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>SUM-Zit/Rahm</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>#-Pub/Groß</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#-Pub/2015/Groß</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$E$3:$E$12</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>126.01299999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>69.328000000000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>105.357</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>286.15899999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70.63000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56.046999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>184.53300000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>53.843000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>94.222000000000008</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>79.174000000000007</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="373448288"/>
-        <c:axId val="373447728"/>
-      </c:lineChart>
       <c:catAx>
-        <c:axId val="373448288"/>
+        <c:axId val="84274144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,14 +923,15 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373447728"/>
+        <c:crossAx val="84274704"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373447728"/>
+        <c:axId val="84274704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +951,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -947,7 +982,8 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373448288"/>
+        <c:crossAx val="84274144"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
       </c:valAx>
@@ -1590,13 +1626,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1882,201 +1918,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E13"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>177.34299999999999</v>
-      </c>
-      <c r="D3" s="11">
-        <v>51.33</v>
-      </c>
-      <c r="E3" s="18">
-        <f>C3-D3</f>
-        <v>126.01299999999999</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>76.878</v>
-      </c>
-      <c r="D4" s="10">
-        <v>7.55</v>
-      </c>
-      <c r="E4" s="22">
-        <f t="shared" ref="E4:E12" si="0">C4-D4</f>
-        <v>69.328000000000003</v>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="20">
+        <v>177.34299999999999</v>
+      </c>
+      <c r="D4" s="21">
+        <v>51.33</v>
+      </c>
+      <c r="E4" s="9">
+        <f>C4-D4</f>
+        <v>126.01299999999999</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="22">
+        <v>76.878</v>
+      </c>
+      <c r="D5" s="23">
+        <v>7.55</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" ref="E5:E13" si="0">C5-D5</f>
+        <v>69.328000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="22">
         <v>120.727</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D6" s="23">
         <v>15.37</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E6" s="12">
         <f t="shared" si="0"/>
         <v>105.357</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="24">
         <v>317.959</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D7" s="25">
         <v>31.8</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>286.15899999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="22">
         <v>70.7</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D8" s="23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E8" s="9">
         <f t="shared" si="0"/>
         <v>70.63000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="22">
         <v>59.756999999999998</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D9" s="23">
         <v>3.71</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E9" s="12">
         <f t="shared" si="0"/>
         <v>56.046999999999997</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="22">
         <v>184.85300000000001</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D10" s="23">
         <v>0.32</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E10" s="12">
         <f t="shared" si="0"/>
         <v>184.53300000000002</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6" t="s">
+    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="24">
         <v>58.633000000000003</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D11" s="25">
         <v>4.79</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E11" s="13">
         <f t="shared" si="0"/>
         <v>53.843000000000004</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="22">
         <v>94.352000000000004</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D12" s="23">
         <v>0.13</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
         <v>94.222000000000008</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
+    <row r="13" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C13" s="26">
         <v>79.254000000000005</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D13" s="27">
         <v>0.08</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E13" s="14">
         <f t="shared" si="0"/>
         <v>79.174000000000007</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+    <row r="14" spans="2:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17">
-        <f>AVERAGE(C3:C12)</f>
+      <c r="C14" s="28">
+        <f>AVERAGE(C4:C13)</f>
         <v>124.04559999999999</v>
       </c>
-      <c r="D13" s="21">
-        <f t="shared" ref="D13:E13" si="1">AVERAGE(D3:D12)</f>
+      <c r="D14" s="29">
+        <f t="shared" ref="D14:E14" si="1">AVERAGE(D4:D13)</f>
         <v>11.514999999999997</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E14" s="15">
         <f t="shared" si="1"/>
         <v>112.53060000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
RESULTS: Changed formatting again.
</commit_message>
<xml_diff>
--- a/documents/bigprak_ergebnisse.xlsx
+++ b/documents/bigprak_ergebnisse.xlsx
@@ -424,15 +424,6 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -443,6 +434,15 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -750,8 +750,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="84274144"/>
-        <c:axId val="84274704"/>
+        <c:axId val="141357616"/>
+        <c:axId val="141358176"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -880,7 +880,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84274144"/>
+        <c:axId val="141357616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +923,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84274704"/>
+        <c:crossAx val="141358176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -931,7 +931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84274704"/>
+        <c:axId val="141358176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +951,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -982,7 +982,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84274144"/>
+        <c:crossAx val="141357616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -1921,7 +1921,7 @@
   <dimension ref="B1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,11 +1938,11 @@
       <c r="B2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
@@ -1960,10 +1960,10 @@
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="17">
         <v>177.34299999999999</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="18">
         <v>51.33</v>
       </c>
       <c r="E4" s="9">
@@ -1975,10 +1975,10 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="19">
         <v>76.878</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="20">
         <v>7.55</v>
       </c>
       <c r="E5" s="12">
@@ -1990,10 +1990,10 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="19">
         <v>120.727</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <v>15.37</v>
       </c>
       <c r="E6" s="12">
@@ -2005,10 +2005,10 @@
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="21">
         <v>317.959</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>31.8</v>
       </c>
       <c r="E7" s="13">
@@ -2020,10 +2020,10 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="19">
         <v>70.7</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E8" s="9">
@@ -2035,10 +2035,10 @@
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="19">
         <v>59.756999999999998</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="20">
         <v>3.71</v>
       </c>
       <c r="E9" s="12">
@@ -2050,10 +2050,10 @@
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="19">
         <v>184.85300000000001</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="20">
         <v>0.32</v>
       </c>
       <c r="E10" s="12">
@@ -2065,10 +2065,10 @@
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <v>58.633000000000003</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>4.79</v>
       </c>
       <c r="E11" s="13">
@@ -2080,10 +2080,10 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="19">
         <v>94.352000000000004</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>0.13</v>
       </c>
       <c r="E12" s="10">
@@ -2095,10 +2095,10 @@
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="23">
         <v>79.254000000000005</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="24">
         <v>0.08</v>
       </c>
       <c r="E13" s="14">
@@ -2110,11 +2110,11 @@
       <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="25">
         <f>AVERAGE(C4:C13)</f>
         <v>124.04559999999999</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="26">
         <f t="shared" ref="D14:E14" si="1">AVERAGE(D4:D13)</f>
         <v>11.514999999999997</v>
       </c>

</xml_diff>